<commit_message>
Work on LMT01 code
</commit_message>
<xml_diff>
--- a/TME CTDB.xlsx
+++ b/TME CTDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlosj\Documents\HARP\Temperature-Measurement-Electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRC\Temperature-Measurement-Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD727F38-6CAE-4D6D-8EE0-580F895181E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38149F7C-788C-4F5A-928F-C9E46BC05574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
+    <workbookView xWindow="25080" yWindow="-75" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="42">
   <si>
     <t>Opcode</t>
   </si>
@@ -108,24 +108,15 @@
     <t>Periodic?</t>
   </si>
   <si>
-    <t>Input Voltage</t>
-  </si>
-  <si>
     <t>Oversize Frame</t>
   </si>
   <si>
     <t>Byte stuffing error</t>
   </si>
   <si>
-    <t>RESERVED</t>
-  </si>
-  <si>
     <t>Test val</t>
   </si>
   <si>
-    <t>0x0201</t>
-  </si>
-  <si>
     <t>Test Val</t>
   </si>
   <si>
@@ -136,6 +127,33 @@
   </si>
   <si>
     <t>Last unhandled interrupt</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Bank A Temps</t>
+  </si>
+  <si>
+    <t>Bank B Temps</t>
+  </si>
+  <si>
+    <t>Bank C Temps</t>
+  </si>
+  <si>
+    <t>TX Buffer High Water Mark</t>
+  </si>
+  <si>
+    <t>0x55</t>
+  </si>
+  <si>
+    <t>0xAA</t>
+  </si>
+  <si>
+    <t>RX Buffer High Water Mark</t>
+  </si>
+  <si>
+    <t>Loop overruns</t>
   </si>
 </sst>
 </file>
@@ -240,18 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -265,15 +271,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -296,6 +293,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15506803-107E-4CEA-AE31-1AE0D93F8418}">
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I132" sqref="I132"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,6 +686,9 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -690,6 +711,9 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -701,6 +725,9 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -720,6 +747,12 @@
       <c r="B9">
         <v>7</v>
       </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -728,6 +761,12 @@
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -735,6 +774,12 @@
       </c>
       <c r="B11">
         <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,16 +2769,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="9.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="11"/>
-    <col min="5" max="5" width="22.5703125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="11"/>
-    <col min="7" max="7" width="14.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="11"/>
-    <col min="9" max="9" width="15.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="25"/>
-    <col min="11" max="11" width="9.140625" style="13"/>
+    <col min="2" max="2" width="9.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="22.5703125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="14.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="7"/>
+    <col min="9" max="9" width="15.42578125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="18"/>
+    <col min="11" max="11" width="9.140625" style="9"/>
     <col min="12" max="12" width="9.140625" style="2"/>
     <col min="13" max="13" width="11.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="2"/>
@@ -2742,64 +2787,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="21" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:15" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="14"/>
+      <c r="C3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -2807,12 +2852,12 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="C4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="14"/>
+      <c r="C4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
@@ -2834,25 +2879,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A02272-D6C1-435F-80C3-C6D3E06E8CAA}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="9.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="12" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="11"/>
-    <col min="12" max="12" width="18.42578125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="7"/>
+    <col min="12" max="12" width="18.42578125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="9" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="3"/>
     <col min="15" max="15" width="14.42578125" style="2" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="3"/>
@@ -2861,110 +2906,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="8" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-    </row>
-    <row r="2" spans="1:20" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+    </row>
+    <row r="2" spans="1:20" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="21" t="s">
+      <c r="J2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="M2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="P2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="10"/>
+      <c r="E3" s="7">
         <v>8</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="F3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7">
         <v>8</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="10">
         <v>8</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="7">
         <v>8</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="10">
         <v>3</v>
       </c>
       <c r="N3" s="4"/>
@@ -2974,30 +3011,30 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="D4" s="14"/>
-      <c r="E4" s="11">
+      <c r="D4" s="10"/>
+      <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="11">
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="7">
         <v>8</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="10">
         <v>7</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="7">
         <v>8</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="10">
         <v>2</v>
       </c>
       <c r="N4" s="4"/>
@@ -3006,26 +3043,31 @@
       <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C5" s="15"/>
-      <c r="D5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="11">
+      <c r="C5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="7">
         <v>8</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="F5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="7">
+        <v>8</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="10">
         <v>6</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="7">
         <v>8</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="10">
         <v>1</v>
       </c>
       <c r="N5" s="4"/>
@@ -3035,28 +3077,21 @@
       <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
-        <v>16</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="11">
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="7">
         <v>8</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="I6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="10">
         <v>5</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="14"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="R6" s="4"/>
@@ -3064,18 +3099,18 @@
       <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="14"/>
-      <c r="H7" s="11">
+      <c r="D7" s="10"/>
+      <c r="H7" s="7">
         <v>8</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="10">
         <v>4</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="14"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -3085,21 +3120,21 @@
       <c r="T7" s="4"/>
     </row>
     <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="15"/>
-      <c r="D8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="11">
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="7">
         <v>8</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="10">
         <v>3</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="14"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -3109,21 +3144,21 @@
       <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="15"/>
-      <c r="D9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="11">
+      <c r="C9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="7">
         <v>8</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="14">
-        <v>2</v>
-      </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="14"/>
+      <c r="J9" s="10">
+        <v>2</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -3133,21 +3168,21 @@
       <c r="T9" s="4"/>
     </row>
     <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="11">
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="7">
         <v>8</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="14">
-        <v>1</v>
-      </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="14"/>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -3156,14 +3191,22 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C11" s="15"/>
-      <c r="D11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="14"/>
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="7">
+        <v>8</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -3172,14 +3215,22 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="14"/>
+    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="7">
+        <v>8</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -3189,14 +3240,14 @@
       <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="14"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="14"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="10"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -3206,14 +3257,14 @@
       <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="14"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="14"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="10"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -3223,14 +3274,13 @@
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="14"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="10"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -3240,14 +3290,14 @@
       <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="14"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="10"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -3257,14 +3307,14 @@
       <c r="T16" s="4"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="14"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="14"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="10"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -3274,14 +3324,14 @@
       <c r="T17" s="4"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="14"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="14"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="14"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="10"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -3291,14 +3341,14 @@
       <c r="T18" s="4"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -3308,14 +3358,14 @@
       <c r="T19" s="4"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="14"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -3325,14 +3375,14 @@
       <c r="T20" s="4"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="14"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="14"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="14"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -3342,14 +3392,14 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="14"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="14"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="14"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="10"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="10"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -3359,14 +3409,14 @@
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="14"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="14"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="14"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="10"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="10"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="10"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -3400,12 +3450,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>